<commit_message>
Add exceldelib and ReinscInsc.
</commit_message>
<xml_diff>
--- a/App/database/nouveauEtudiant.xlsx
+++ b/App/database/nouveauEtudiant.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Housni Achbouq\Downloads\My-Github\JAVA project\Design-and-Development-of-a-Notes-Management-Java-Application\App\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Housni Achbouq\Downloads\My-Github\benabbou work\Design-and-Development-of-a-Notes-Management-Java-Application\App\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A33BC02-CFC3-4C2E-A409-2998BC6BDF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E474417D-FA14-436D-A72C-197D4F7CA26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2388" windowWidth="21264" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Emp Info" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>ID ETUDIANT</t>
   </si>
@@ -40,34 +40,64 @@
     <t>TYPE</t>
   </si>
   <si>
+    <t>J133341333</t>
+  </si>
+  <si>
+    <t>Lfelous</t>
+  </si>
+  <si>
+    <t>Rim</t>
+  </si>
+  <si>
     <t>Achbouq</t>
   </si>
   <si>
     <t>Housni</t>
   </si>
   <si>
-    <t>Bennabou</t>
-  </si>
-  <si>
-    <t>Oussama</t>
-  </si>
-  <si>
-    <t>J133341333</t>
-  </si>
-  <si>
-    <t>S133341333</t>
+    <t>INSCRIPTION</t>
   </si>
   <si>
     <t>K133341333</t>
   </si>
   <si>
-    <t>Lfelous</t>
-  </si>
-  <si>
-    <t>Rim</t>
-  </si>
-  <si>
-    <t>INSCRIPTION</t>
+    <t>M133341333</t>
+  </si>
+  <si>
+    <t>REINSCRIPTION</t>
+  </si>
+  <si>
+    <t>Benabbou2</t>
+  </si>
+  <si>
+    <t>Oussama2</t>
+  </si>
+  <si>
+    <t>A133341333</t>
+  </si>
+  <si>
+    <t>B133341333</t>
+  </si>
+  <si>
+    <t>C133341333</t>
+  </si>
+  <si>
+    <t>Yamani</t>
+  </si>
+  <si>
+    <t>Jamal</t>
+  </si>
+  <si>
+    <t>Ferdous</t>
+  </si>
+  <si>
+    <t>Kamal</t>
+  </si>
+  <si>
+    <t>Touhami</t>
+  </si>
+  <si>
+    <t>Badr</t>
   </si>
 </sst>
 </file>
@@ -422,7 +452,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,19 +488,19 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -478,19 +508,19 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -498,24 +528,81 @@
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
+    </row>
+    <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>15</v>
+      <c r="F5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update log4j and maven dependency.
</commit_message>
<xml_diff>
--- a/App/database/nouveauEtudiant.xlsx
+++ b/App/database/nouveauEtudiant.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Housni Achbouq\Desktop\Design-and-Development-of-a-Notes-Management-Java-Application\App\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Housni Achbouq\Desktop\tests\step2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDBC179-9206-4852-AD5C-E965C5C1F5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D2F627-DB27-4B1A-8124-3F6760751B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="876" yWindow="504" windowWidth="21936" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Emp Info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>ID ETUDIANT</t>
   </si>
@@ -61,13 +61,43 @@
     <t>K133341333</t>
   </si>
   <si>
-    <t>Benabbou</t>
-  </si>
-  <si>
-    <t>Oussama</t>
-  </si>
-  <si>
     <t>M133341333</t>
+  </si>
+  <si>
+    <t>REINSCRIPTION</t>
+  </si>
+  <si>
+    <t>Benabbou2</t>
+  </si>
+  <si>
+    <t>Oussama2</t>
+  </si>
+  <si>
+    <t>A133341333</t>
+  </si>
+  <si>
+    <t>B133341333</t>
+  </si>
+  <si>
+    <t>C133341333</t>
+  </si>
+  <si>
+    <t>Yamani</t>
+  </si>
+  <si>
+    <t>Jamal</t>
+  </si>
+  <si>
+    <t>Ferdous</t>
+  </si>
+  <si>
+    <t>Kamal</t>
+  </si>
+  <si>
+    <t>Touhami</t>
+  </si>
+  <si>
+    <t>Badr</t>
   </si>
 </sst>
 </file>
@@ -422,7 +452,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,10 +497,10 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -481,16 +511,16 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -498,7 +528,7 @@
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -507,15 +537,72 @@
         <v>8</v>
       </c>
       <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>